<commit_message>
Update journal entry overall preview screen
</commit_message>
<xml_diff>
--- a/Documentation/Project Progress Document.xlsx
+++ b/Documentation/Project Progress Document.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\Working-Space\Ship-Journal\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191B78E5-BFBE-4613-AA8E-FC1CA71BD26D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA53668-CC1E-4D11-AD82-C37AE5BFF44C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{C93F7B9C-8EB9-402E-AA39-1D20BFE1AF91}"/>
   </bookViews>
   <sheets>
     <sheet name="Functional Requirements" sheetId="1" r:id="rId1"/>
+    <sheet name="Non-Functional Requirements" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -24,9 +25,158 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
+  <si>
+    <t>Screen</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Function</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Change language</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Navigate to other screen/ Choose menu</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>English/Japanese options when clicking on dropdown menu at the bottom-left corner</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Navigate to according screen when clicking on menu</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Select date</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Third Layer Screen</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Select person on duty</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Select moment</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Select name in the dropdown menu</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Select moment by 2hrs step (exmaple: 0:00, 2:00, 4:00)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Fourth Layer Screen</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Fifth Layer Screen</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>List preview of 4 grid views of 4 entry parameters (M/E, A/E, REF, TEMP)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Input comment</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>As function name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Type comment in the input field</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Home - First Layer Screen</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Date Screen - Second Layer Screen</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Select comment to view</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Select comment from dropdown menu</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Input item name and quantity/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Item name as string. Quantity/Value as numeric</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Select date by format dd//mm//yyyy</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Return</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Return to previous screen - Fifth layer screen</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Save the data in the grid and navigate to overal grid preview screen</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>TEMP grid view - Input screen</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>REF grid view - Input screen</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>A/E grid view - Input screen</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>M/E grid view - Input screen</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Overall grid preview</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Save the data in the grid and navigate to overall grid preview screen</t>
+    <phoneticPr fontId="1"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -42,6 +192,24 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -51,7 +219,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -59,15 +227,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -383,11 +627,351 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{844AE880-746F-474C-8BA1-CCE0F469AFB0}">
+  <dimension ref="A1:C36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="34" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="75.25" style="6" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="12"/>
+      <c r="B3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="13"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
+    </row>
+    <row r="5" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="13"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+    </row>
+    <row r="7" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="12"/>
+      <c r="B8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="13"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+    </row>
+    <row r="10" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="13"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+    </row>
+    <row r="12" spans="1:3" ht="38.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="12"/>
+      <c r="B13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="13"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+    </row>
+    <row r="15" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="15"/>
+      <c r="B16" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="15"/>
+      <c r="B17" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="15"/>
+      <c r="B18" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="16"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="9"/>
+    </row>
+    <row r="20" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="15"/>
+      <c r="B21" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="15"/>
+      <c r="B22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="15"/>
+      <c r="B23" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="16"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="9"/>
+    </row>
+    <row r="25" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="15"/>
+      <c r="B26" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="15"/>
+      <c r="B27" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="15"/>
+      <c r="B28" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A29" s="16"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="9"/>
+    </row>
+    <row r="30" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A30" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="15"/>
+      <c r="B31" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="15"/>
+      <c r="B32" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A33" s="15"/>
+      <c r="B33" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="16"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="9"/>
+    </row>
+    <row r="35" spans="1:3" ht="38.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="15"/>
+      <c r="B36" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A30:A33"/>
+  </mergeCells>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9F15FA0-2831-49AF-967B-E1BED55FE3E0}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <sheetData/>

</xml_diff>

<commit_message>
Complete updating preview screen in watch menu selection screen
</commit_message>
<xml_diff>
--- a/Documentation/Project Progress Document.xlsx
+++ b/Documentation/Project Progress Document.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\Working-Space\Ship-Journal\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA53668-CC1E-4D11-AD82-C37AE5BFF44C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2823EB3B-6DFB-47B6-A8B1-2D870DF60786}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{C93F7B9C-8EB9-402E-AA39-1D20BFE1AF91}"/>
   </bookViews>
@@ -629,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{844AE880-746F-474C-8BA1-CCE0F469AFB0}">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>

</xml_diff>